<commit_message>
added 23 command in this file
</commit_message>
<xml_diff>
--- a/git&github command.xlsx
+++ b/git&github command.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunil-IT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2090B785-A0B0-44AC-8713-EF06C926405D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45D0CCD-CD50-4BD7-84E1-C371702E3F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={142EC051-72A3-4E7B-9C46-C7E8260899CE}</author>
+  </authors>
+  <commentList>
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{142EC051-72A3-4E7B-9C46-C7E8260899CE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    First check our deleted file are showing are not we can check it with (git status) command if we find deleted file is showing here then we can restore it with git restore command</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>S.No.</t>
   </si>
@@ -83,9 +101,6 @@
     <t>git remote  -v</t>
   </si>
   <si>
-    <t>git remote set-url origin https:// PAT TOKEN @git repository address</t>
-  </si>
-  <si>
     <t>git config --global user.name  "your user name"</t>
   </si>
   <si>
@@ -108,19 +123,136 @@
   </si>
   <si>
     <t>Git Related Commands</t>
+  </si>
+  <si>
+    <t>git restore --staged file_name</t>
+  </si>
+  <si>
+    <t>for rollback from staged to untracked area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for remove the file </t>
+  </si>
+  <si>
+    <t>rm file name</t>
+  </si>
+  <si>
+    <t>git restore file name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To restore deleted file from git </t>
+  </si>
+  <si>
+    <t>git checkout any branch</t>
+  </si>
+  <si>
+    <t>To switch on perticular branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git checkout -b Any new branch name </t>
+  </si>
+  <si>
+    <t>To Create a new from from this existing branch and switch on new branch</t>
+  </si>
+  <si>
+    <t>To remove any perticular branch</t>
+  </si>
+  <si>
+    <t>git branch -d any branch name</t>
+  </si>
+  <si>
+    <t>To show remote origin URL</t>
+  </si>
+  <si>
+    <t>git remote add origin (remote git URL)</t>
+  </si>
+  <si>
+    <t>To add remote Origin Url</t>
+  </si>
+  <si>
+    <t>git remote remove origin</t>
+  </si>
+  <si>
+    <t>To remove remote origin url</t>
+  </si>
+  <si>
+    <t>git remote set-url origin 'https:// PAT TOKEN @git repository address'</t>
+  </si>
+  <si>
+    <t>git fetch</t>
+  </si>
+  <si>
+    <t>To fetch the all branches from remote to local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git clone </t>
+  </si>
+  <si>
+    <r>
+      <t>GIT_SSH_COMMAND="ssh -i /home/ubuntu/.ssh/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> your private key"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> git clone </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>your ssh clone url address</t>
+    </r>
+  </si>
+  <si>
+    <t>To use any perticular ssh private key instead of Default ssh private key for ssh git clone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,6 +295,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Sunil Prajapati" id="{44188E45-5BEC-4FC0-97A4-49CCC09B3279}" userId="S::sunil.prajapati@vivogujarat.com::2a6b74ed-6efe-4867-bbd5-f077cfd6242a" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,19 +618,27 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C15" dT="2024-02-17T15:42:59.09" personId="{44188E45-5BEC-4FC0-97A4-49CCC09B3279}" id="{142EC051-72A3-4E7B-9C46-C7E8260899CE}">
+    <text>First check our deleted file are showing are not we can check it with (git status) command if we find deleted file is showing here then we can restore it with git restore command</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -579,16 +725,19 @@
       <c r="B8" t="s">
         <v>14</v>
       </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,10 +745,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,10 +756,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,7 +767,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,15 +775,130 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>